<commit_message>
Added stage 5,6 pdf and edited code
</commit_message>
<xml_diff>
--- a/code/ALGS-DATASET-AUCS+RANKS.xlsx
+++ b/code/ALGS-DATASET-AUCS+RANKS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ipism\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ipism\Desktop\Applied-ML\odin\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C4B6AE7-96E5-4EF3-9C53-7C7D692A54B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCE9D07-9DCF-457F-9DEF-AA0AF095EDBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{532F0C35-8739-4353-8C38-AD9ACCA9AAED}"/>
   </bookViews>
@@ -19,7 +19,6 @@
     <externalReference r:id="rId2"/>
   </externalReferences>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -217,6 +216,32 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{378F0EAF-2CE3-40EF-9B09-BF13DE9F6766}" name="Table1" displayName="Table1" ref="A1:D21" totalsRowShown="0">
+  <autoFilter ref="A1:D21" xr:uid="{378F0EAF-2CE3-40EF-9B09-BF13DE9F6766}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{B813E762-4C69-4E98-9230-BF0533C43A92}" name="DATASET"/>
+    <tableColumn id="2" xr3:uid="{5ADDEB4D-DA12-46D7-A445-9F931A9FB174}" name="ALG1"/>
+    <tableColumn id="3" xr3:uid="{4FF39264-EC26-44FD-9CAA-CD10113CD090}" name="ALG2"/>
+    <tableColumn id="4" xr3:uid="{5DF3ADED-E6D4-46DF-810A-BEDA22D7DDF8}" name="ALG3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DD74441C-E178-4AF9-9953-C2604403542C}" name="Table2" displayName="Table2" ref="G1:J21" totalsRowShown="0">
+  <autoFilter ref="G1:J21" xr:uid="{DD74441C-E178-4AF9-9953-C2604403542C}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{0A08E4E0-81BE-441A-A6DC-731788C0D45B}" name="DATASET"/>
+    <tableColumn id="2" xr3:uid="{5921D7E9-BAB3-49F0-A422-CE9763069A4A}" name="ALG1"/>
+    <tableColumn id="3" xr3:uid="{512F8000-6828-4F58-9662-3932A32CB429}" name="ALG2"/>
+    <tableColumn id="4" xr3:uid="{0DB3A146-824C-430E-9B5A-7CDAB2A94C0B}" name="ALG3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -519,10 +544,14 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="10.1796875" customWidth="1"/>
+    <col min="7" max="7" width="10.1796875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
@@ -1087,5 +1116,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>